<commit_message>
Final update for SIAL
</commit_message>
<xml_diff>
--- a/phylogenies/Species_information.xlsx
+++ b/phylogenies/Species_information.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jax/🔬Research/2024 - fungal_annotations/phylogenies/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jax/🔬Research/2024 - fungal_annotations/fungal_sRNA_annotations/phylogenies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA97CD4E-8435-F440-A12F-078C6B7DC860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E37F10D-3CD3-A347-816B-2D08390573AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="880" yWindow="1540" windowWidth="28800" windowHeight="18000" xr2:uid="{063D12AA-F3DC-8D49-A3A0-2F44CA381166}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="326">
   <si>
     <t>Ascosphaera apis</t>
   </si>
@@ -999,6 +999,21 @@
   </si>
   <si>
     <t>Paracoccidioides brasiliensis</t>
+  </si>
+  <si>
+    <t>clean_lifestyle</t>
+  </si>
+  <si>
+    <t>Plant pathogen</t>
+  </si>
+  <si>
+    <t>Insect pathogen</t>
+  </si>
+  <si>
+    <t>Human pathogen</t>
+  </si>
+  <si>
+    <t>Carnivore</t>
   </si>
 </sst>
 </file>
@@ -1101,12 +1116,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{55A210D0-23B2-1848-88B1-CAF0C9FABBF7}" name="Table1" displayName="Table1" ref="A1:M94" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:M94" xr:uid="{55A210D0-23B2-1848-88B1-CAF0C9FABBF7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{55A210D0-23B2-1848-88B1-CAF0C9FABBF7}" name="Table1" displayName="Table1" ref="A1:N94" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:N94" xr:uid="{55A210D0-23B2-1848-88B1-CAF0C9FABBF7}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M94">
     <sortCondition ref="B1:B94"/>
   </sortState>
-  <tableColumns count="13">
+  <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{0D024533-DFA7-0A4F-84DF-71D2BDC7E5AB}" name="Species"/>
     <tableColumn id="2" xr3:uid="{E407CE3A-359A-AB49-BCC5-B7382695A463}" name="Code"/>
     <tableColumn id="3" xr3:uid="{EDF4164E-2C99-7B4A-A465-7C603F6ED213}" name="AKA"/>
@@ -1120,6 +1135,7 @@
     <tableColumn id="11" xr3:uid="{BC734CC4-696D-714B-B88E-4DA1CBC48C07}" name="Sources"/>
     <tableColumn id="12" xr3:uid="{FCEF48AB-5915-8445-8AE2-002D0C8C6462}" name="Information Level"/>
     <tableColumn id="13" xr3:uid="{B38FFA27-E410-C941-A3AC-505CEE7FCB1B}" name="lifestyle"/>
+    <tableColumn id="14" xr3:uid="{32C2864C-DD45-0D4C-8AA4-B1B1975B35AB}" name="clean_lifestyle"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1422,11 +1438,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFB3DC3A-733E-BE49-BA0B-7ED842D78587}">
-  <dimension ref="A1:M94"/>
+  <dimension ref="A1:N94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A70" sqref="A70:XFD70"/>
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N94" sqref="N94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1443,7 +1459,7 @@
     <col min="12" max="12" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>45</v>
       </c>
@@ -1483,8 +1499,11 @@
       <c r="M1" s="3" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N1" s="3" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>251</v>
       </c>
@@ -1497,8 +1516,11 @@
       <c r="M2" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>193</v>
       </c>
@@ -1529,8 +1551,11 @@
       <c r="L3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N3" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>194</v>
       </c>
@@ -1558,8 +1583,11 @@
       <c r="L4" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N4" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1590,8 +1618,11 @@
       <c r="L5" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N5" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>195</v>
       </c>
@@ -1619,8 +1650,11 @@
       <c r="L6" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -1651,8 +1685,11 @@
       <c r="L7" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N7" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>252</v>
       </c>
@@ -1668,8 +1705,11 @@
       <c r="M8" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N8" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -1700,8 +1740,11 @@
       <c r="L9" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N9" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>253</v>
       </c>
@@ -1714,8 +1757,11 @@
       <c r="M10" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N10" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>196</v>
       </c>
@@ -1746,8 +1792,11 @@
       <c r="L11" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N11" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>197</v>
       </c>
@@ -1781,8 +1830,11 @@
       <c r="L12" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N12" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>254</v>
       </c>
@@ -1798,8 +1850,11 @@
       <c r="M13" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N13" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -1833,8 +1888,11 @@
       <c r="L14" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N14" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -1865,8 +1923,11 @@
       <c r="L15" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N15" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>255</v>
       </c>
@@ -1882,8 +1943,11 @@
       <c r="M16" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N16" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -1917,8 +1981,11 @@
       <c r="L17" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N17" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>256</v>
       </c>
@@ -1931,8 +1998,11 @@
       <c r="I18" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N18" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>257</v>
       </c>
@@ -1948,8 +2018,11 @@
       <c r="M19" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N19" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>258</v>
       </c>
@@ -1962,8 +2035,11 @@
       <c r="M20" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N20" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -1997,8 +2073,11 @@
       <c r="M21" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N21" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>198</v>
       </c>
@@ -2029,8 +2108,11 @@
       <c r="L22" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N22" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>199</v>
       </c>
@@ -2064,8 +2146,11 @@
       <c r="L23" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N23" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -2096,8 +2181,11 @@
       <c r="L24" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N24" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -2131,8 +2219,11 @@
       <c r="L25" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N25" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>259</v>
       </c>
@@ -2148,8 +2239,11 @@
       <c r="M26" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N26" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>260</v>
       </c>
@@ -2162,8 +2256,11 @@
       <c r="I27" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N27" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -2194,8 +2291,11 @@
       <c r="L28" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N28" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>261</v>
       </c>
@@ -2208,8 +2308,11 @@
       <c r="I29" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N29" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>200</v>
       </c>
@@ -2240,8 +2343,11 @@
       <c r="L30" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N30" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>262</v>
       </c>
@@ -2254,8 +2360,11 @@
       <c r="I31" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N31" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>201</v>
       </c>
@@ -2289,8 +2398,11 @@
       <c r="L32" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N32" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>263</v>
       </c>
@@ -2303,8 +2415,11 @@
       <c r="I33" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N33" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>10</v>
       </c>
@@ -2338,8 +2453,11 @@
       <c r="L34" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N34" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>11</v>
       </c>
@@ -2370,8 +2488,11 @@
       <c r="L35" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N35" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>12</v>
       </c>
@@ -2402,8 +2523,11 @@
       <c r="L36" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N36" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>13</v>
       </c>
@@ -2437,8 +2561,11 @@
       <c r="M37" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N37" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>14</v>
       </c>
@@ -2469,8 +2596,11 @@
       <c r="M38" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N38" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>15</v>
       </c>
@@ -2504,8 +2634,11 @@
       <c r="L39" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N39" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>16</v>
       </c>
@@ -2539,8 +2672,11 @@
       <c r="M40" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N40" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>17</v>
       </c>
@@ -2571,8 +2707,11 @@
       <c r="L41" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N41" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>264</v>
       </c>
@@ -2585,8 +2724,11 @@
       <c r="I42" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N42" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>319</v>
       </c>
@@ -2623,8 +2765,11 @@
       <c r="L43" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N43" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>18</v>
       </c>
@@ -2655,8 +2800,11 @@
       <c r="L44" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N44" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>265</v>
       </c>
@@ -2672,8 +2820,11 @@
       <c r="I45" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N45" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>19</v>
       </c>
@@ -2707,8 +2858,11 @@
       <c r="L46" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N46" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>20</v>
       </c>
@@ -2739,8 +2893,11 @@
       <c r="L47" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N47" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>266</v>
       </c>
@@ -2753,8 +2910,11 @@
       <c r="M48" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N48" s="2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>21</v>
       </c>
@@ -2788,8 +2948,11 @@
       <c r="M49" s="2" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N49" s="2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>22</v>
       </c>
@@ -2820,8 +2983,11 @@
       <c r="M50" s="2" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N50" s="2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>267</v>
       </c>
@@ -2837,8 +3003,11 @@
       <c r="I51" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N51" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>23</v>
       </c>
@@ -2869,8 +3038,11 @@
       <c r="L52" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N52" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>268</v>
       </c>
@@ -2886,8 +3058,11 @@
       <c r="I53" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N53" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>320</v>
       </c>
@@ -2918,8 +3093,11 @@
       <c r="L54" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N54" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>24</v>
       </c>
@@ -2950,8 +3128,11 @@
       <c r="L55" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N55" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>25</v>
       </c>
@@ -2979,8 +3160,11 @@
       <c r="M56" s="2" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N56" s="2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>26</v>
       </c>
@@ -3008,8 +3192,11 @@
       <c r="L57" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N57" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>269</v>
       </c>
@@ -3022,8 +3209,11 @@
       <c r="I58" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N58" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>270</v>
       </c>
@@ -3036,8 +3226,11 @@
       <c r="M59" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N59" s="2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>27</v>
       </c>
@@ -3062,9 +3255,6 @@
       <c r="H60" t="s">
         <v>144</v>
       </c>
-      <c r="I60" t="s">
-        <v>99</v>
-      </c>
       <c r="J60" t="s">
         <v>96</v>
       </c>
@@ -3077,8 +3267,11 @@
       <c r="M60" s="2" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N60" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>28</v>
       </c>
@@ -3112,8 +3305,11 @@
       <c r="M61" s="2" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N61" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>202</v>
       </c>
@@ -3126,8 +3322,11 @@
       <c r="M62" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N62" s="2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>203</v>
       </c>
@@ -3155,8 +3354,11 @@
       <c r="L63" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N63" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>271</v>
       </c>
@@ -3169,8 +3371,11 @@
       <c r="I64" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N64" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>29</v>
       </c>
@@ -3204,8 +3409,11 @@
       <c r="L65" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N65" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>272</v>
       </c>
@@ -3218,8 +3426,11 @@
       <c r="I66" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N66" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>204</v>
       </c>
@@ -3253,8 +3464,11 @@
       <c r="M67" s="2" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N67" s="2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>273</v>
       </c>
@@ -3267,8 +3481,11 @@
       <c r="M68" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N68" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>30</v>
       </c>
@@ -3302,8 +3519,11 @@
       <c r="M69" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N69" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>274</v>
       </c>
@@ -3316,8 +3536,11 @@
       <c r="M70" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N70" s="2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>31</v>
       </c>
@@ -3351,8 +3574,11 @@
       <c r="L71" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N71" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>32</v>
       </c>
@@ -3383,8 +3609,11 @@
       <c r="L72" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N72" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>205</v>
       </c>
@@ -3415,8 +3644,11 @@
       <c r="M73" s="2" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N73" s="2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>33</v>
       </c>
@@ -3450,8 +3682,11 @@
       <c r="M74" s="2" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N74" s="2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>275</v>
       </c>
@@ -3464,8 +3699,11 @@
       <c r="M75" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N75" s="2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>34</v>
       </c>
@@ -3499,8 +3737,11 @@
       <c r="M76" s="2" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N76" s="2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>35</v>
       </c>
@@ -3534,8 +3775,11 @@
       <c r="M77" s="2" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N77" s="2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>36</v>
       </c>
@@ -3569,8 +3813,11 @@
       <c r="L78" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N78" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>206</v>
       </c>
@@ -3601,8 +3848,11 @@
       <c r="L79" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N79" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>37</v>
       </c>
@@ -3642,8 +3892,11 @@
       <c r="M80" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N80" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>38</v>
       </c>
@@ -3680,8 +3933,11 @@
       <c r="L81" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N81" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>39</v>
       </c>
@@ -3715,8 +3971,11 @@
       <c r="M82" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N82" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>40</v>
       </c>
@@ -3747,8 +4006,11 @@
       <c r="M83" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N83" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>41</v>
       </c>
@@ -3782,8 +4044,11 @@
       <c r="M84" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N84" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>42</v>
       </c>
@@ -3820,8 +4085,11 @@
       <c r="L85" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N85" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>43</v>
       </c>
@@ -3858,8 +4126,11 @@
       <c r="L86" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N86" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>207</v>
       </c>
@@ -3890,8 +4161,11 @@
       <c r="M87" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N87" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>276</v>
       </c>
@@ -3904,8 +4178,11 @@
       <c r="I88" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N88" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>277</v>
       </c>
@@ -3918,8 +4195,11 @@
       <c r="I89" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N89" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>208</v>
       </c>
@@ -3950,8 +4230,11 @@
       <c r="L90" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N90" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>278</v>
       </c>
@@ -3964,8 +4247,11 @@
       <c r="I91" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N91" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>279</v>
       </c>
@@ -3978,8 +4264,11 @@
       <c r="M92" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N92" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>280</v>
       </c>
@@ -3992,8 +4281,11 @@
       <c r="M93" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N93" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>44</v>
       </c>
@@ -4029,6 +4321,9 @@
       </c>
       <c r="L94" t="s">
         <v>45</v>
+      </c>
+      <c r="N94" t="s">
+        <v>322</v>
       </c>
     </row>
   </sheetData>

</xml_diff>